<commit_message>
Updates for github-pages site
</commit_message>
<xml_diff>
--- a/data/FLRT_survey.xlsx
+++ b/data/FLRT_survey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanhardison/Documents/git/trash_proj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanhardison/Documents/git/FLRT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE71281-A7D5-E040-98E7-A282E15E0EA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F3DB34E-6277-E74C-B0BB-F6A115E92160}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="460" windowWidth="19900" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16660" yWindow="460" windowWidth="21740" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work Plan" sheetId="2" r:id="rId1"/>
@@ -39,20 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>_Deposit legislation                    _More water stations                          _Promote refillable bottles                 _Promote quality of Falmouth H2O       _'Buy it' as cleanup incentive</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Currier Rd. from 135 Regis to Sandwich &amp; back</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sandwich Rd. &amp; Currier to Town Line</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Plastic Bottles - nips</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -141,18 +133,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>WHR GG to KH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NB Ramp to Rt28 from Brick Kiln starting at Evacuation Rt. Sign</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WHR &amp; Locust St. from Greengate to Palmer Ave</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>PLASTIC - all sizes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -279,59 +259,14 @@
     <t>Weight (lbs)</t>
   </si>
   <si>
-    <t>Locust/Main to WH/Kettle Hole Rd.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>WHR Centenniel to 1st driveway going north</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>53 Two Ponds to WHR to St.Barnabas - both sides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sippewissett Rd.-Beccles to Woodneck</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cross St. from Waquoit Farms to Carriage Shop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cross St. from Waquoit Farms to Barrows</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Barrows from Cross St. to Rt. 28</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shore St. full length &amp; both sides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>cigarette packs &amp; butts / cigar plastic tips/                      e-cigarette paraphernalia /paper</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>53 Two Ponds to Greengate intersctn of WHR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WHR @ Greengate, Locust, Main to Estia Rstrnt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Davisville Road from Alwardt Ln to Seashell Ln.</t>
-  </si>
-  <si>
-    <t>Sippowisett Rd -  Ransom to Quissett Harbor Rd.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sippowessett Rd - Beccles to Burnham </t>
-  </si>
-  <si>
     <t>Residential trash</t>
   </si>
   <si>
@@ -351,13 +286,67 @@
   </si>
   <si>
     <t>cups</t>
+  </si>
+  <si>
+    <t>53_Two_Ponds_to_Greengate_intersctn_of_WHR</t>
+  </si>
+  <si>
+    <t>53_Two_Ponds_to_WHR_to_St.Barnabas_-_both_sides</t>
+  </si>
+  <si>
+    <t>Barrows_from_Cross_St._to_Rt._28</t>
+  </si>
+  <si>
+    <t>Cross_St._from_Waquoit_Farms_to_Barrows</t>
+  </si>
+  <si>
+    <t>Cross_St._from_Waquoit_Farms_to_Carriage_Shop</t>
+  </si>
+  <si>
+    <t>LocustMain_to_WHKettle_Hole_Rd.</t>
+  </si>
+  <si>
+    <t>NB_Ramp_to_Rt28_from_Brick_Kiln_starting_at_Evacuation_Rt._Sign</t>
+  </si>
+  <si>
+    <t>Sandwich_Rd._Currier_to_Town_Line</t>
+  </si>
+  <si>
+    <t>Shore_St._full_length_both_sides</t>
+  </si>
+  <si>
+    <t>Sippewissett_Rd.-Beccles_to_Woodneck</t>
+  </si>
+  <si>
+    <t>Sippewissett_Rd.-Beccles_to_Woodneck2</t>
+  </si>
+  <si>
+    <t>Sippowessett_Rd_-_Beccles_to_Burnham</t>
+  </si>
+  <si>
+    <t>Sippowisett_Rd_-__Ransom_to_Quissett_Harbor_Rd.</t>
+  </si>
+  <si>
+    <t>WHR_GG_to_KH</t>
+  </si>
+  <si>
+    <t>WHR_Greengate,_Locust,_Main_to_Estia_Rstrnt</t>
+  </si>
+  <si>
+    <t>WHR_Locust_St._from_Greengate_to_Palmer_Ave</t>
+  </si>
+  <si>
+    <t>Davisville_Road_from_Alwardt_Ln_to_Seashell_Ln.</t>
+  </si>
+  <si>
+    <t>Currier_Rd._from_135_Regis_to_Sandwich_back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1302,7 +1291,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -1312,59 +1301,59 @@
     <col min="6" max="6" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:6" s="8" customFormat="1" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" thickBot="1"/>
+    <row r="2" spans="1:6" s="8" customFormat="1" ht="42" thickTop="1" thickBot="1">
       <c r="A2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="20" t="s">
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" thickTop="1">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="F3" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>0</v>
@@ -1373,27 +1362,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1403,7 +1392,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1413,7 +1402,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1423,7 +1412,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1433,7 +1422,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="72" customHeight="1">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1443,7 +1432,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="72" customHeight="1">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1453,7 +1442,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="72" customHeight="1">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1463,7 +1452,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="72" customHeight="1">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1473,7 +1462,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="72" customHeight="1">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1483,7 +1472,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="72" customHeight="1">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -1514,11 +1503,11 @@
   </sheetPr>
   <dimension ref="A1:AC1048313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:X1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="2" width="24.1640625" style="31" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
@@ -1529,9 +1518,9 @@
     <col min="22" max="22" width="11.1640625" style="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="24" customHeight="1" thickTop="1">
       <c r="A1" s="32" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="34"/>
@@ -1600,70 +1589,70 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="140" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="160">
       <c r="A2" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F2" s="71" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="K2" s="40" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L2" s="40" t="s">
         <v>66</v>
       </c>
       <c r="M2" s="40" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="N2" s="40" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="O2" s="40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P2" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="44" t="s">
-        <v>26</v>
-      </c>
       <c r="S2" s="44" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="U2" s="44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="V2" s="58" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1673,13 +1662,13 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:29" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="24" customHeight="1" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="81"/>
       <c r="C3" s="24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="41">
         <v>1.1000000000000001</v>
@@ -1744,13 +1733,13 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:29" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="24" customHeight="1" thickBot="1">
       <c r="A4" s="26" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B4" s="81"/>
       <c r="C4" s="23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D4" s="45">
         <v>5.6</v>
@@ -1799,15 +1788,15 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="24" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -1847,15 +1836,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="24" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
@@ -1901,15 +1890,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="24" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -1949,15 +1938,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="24" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -2001,15 +1990,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="24" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="37">
         <v>24</v>
@@ -2069,15 +2058,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="24" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="37">
         <v>5</v>
@@ -2125,15 +2114,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="24" customHeight="1">
       <c r="A11" s="28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -2175,15 +2164,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="24" customHeight="1">
       <c r="A12" s="28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -2219,15 +2208,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="28" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D13" s="37">
         <v>4</v>
@@ -2281,15 +2270,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="24" customHeight="1">
       <c r="A14" s="28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
@@ -2329,15 +2318,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="24" customHeight="1">
       <c r="A15" s="28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" s="37">
         <v>5</v>
@@ -2393,15 +2382,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="24" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="37">
         <v>7</v>
@@ -2457,15 +2446,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="24" customHeight="1">
       <c r="A17" s="28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
@@ -2503,15 +2492,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="40">
       <c r="A18" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" s="37">
         <v>4</v>
@@ -2559,15 +2548,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="24" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
@@ -2607,15 +2596,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="24" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -2651,15 +2640,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="24" customHeight="1">
       <c r="A21" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D21" s="37">
         <v>11</v>
@@ -2719,12 +2708,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="24" customHeight="1">
       <c r="A22" s="28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="51">
@@ -2769,12 +2758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="24" customHeight="1">
       <c r="A23" s="28" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="51">
@@ -2821,12 +2810,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="24" customHeight="1">
       <c r="A24" s="28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="51">
@@ -2873,12 +2862,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="24" customHeight="1">
       <c r="A25" s="28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="51"/>
@@ -2921,12 +2910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="24" customHeight="1">
       <c r="A26" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="51">
@@ -2977,9 +2966,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="21" customFormat="1" ht="24" customHeight="1">
       <c r="A27" s="29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="22"/>
@@ -3023,9 +3012,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="24" customHeight="1" thickBot="1">
       <c r="A28" s="28" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="4"/>
@@ -3077,9 +3066,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="24" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="4"/>
@@ -3135,13 +3124,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="92" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" ht="92" customHeight="1" thickTop="1">
       <c r="A30" s="35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="35"/>
       <c r="C30" s="36" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D30" s="53">
         <v>2</v>
@@ -3189,25 +3178,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="30"/>
       <c r="B32" s="30"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="1048312" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="1048312" spans="6:6">
       <c r="F1048312" s="38"/>
     </row>
-    <row r="1048313" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="1048313" spans="6:6">
       <c r="F1048313" s="38"/>
     </row>
   </sheetData>

</xml_diff>